<commit_message>
Species Richness plot + updates
</commit_message>
<xml_diff>
--- a/DATA/TraitDataFrame.xlsx
+++ b/DATA/TraitDataFrame.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roell\OneDrive\Bureaublad\INFC-functional-diversity\Collaboration\raw_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\angelo\Google Drive UNIBAS\Lammerant_et_al\INFC-functional-diversity\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA60D60B-6E7F-4C72-B234-B8F7686ED940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AC9190-90F6-4754-8370-412EC22B6A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="8" xr2:uid="{0BADCDCF-2DCA-4EDE-9EAC-A9D93B18F6A7}"/>
+    <workbookView xWindow="960" yWindow="1995" windowWidth="23340" windowHeight="13755" firstSheet="4" activeTab="8" xr2:uid="{0BADCDCF-2DCA-4EDE-9EAC-A9D93B18F6A7}"/>
   </bookViews>
   <sheets>
     <sheet name="VesselDiameter" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4266" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4102" uniqueCount="622">
   <si>
     <t>Species Code</t>
   </si>
@@ -1537,9 +1537,6 @@
     <t>0-100</t>
   </si>
   <si>
-    <t>na</t>
-  </si>
-  <si>
     <t>-2.6</t>
   </si>
   <si>
@@ -1877,6 +1874,48 @@
   </si>
   <si>
     <t>Kattge J, Knorr W, Raddatz T, Wirth C. 2009. Quantifying photosynthetic capacity and its relatioship to leaf nitrogen content for global-scale terrestrial biosphere models. Global Change Biology 15:976-991.</t>
+  </si>
+  <si>
+    <t>Species me</t>
+  </si>
+  <si>
+    <t>Pinus excelsa (p. wallichia)</t>
+  </si>
+  <si>
+    <t>Pinus pister</t>
+  </si>
+  <si>
+    <t>Pinus uncita</t>
+  </si>
+  <si>
+    <t>Chamaecyparis lawsonia</t>
+  </si>
+  <si>
+    <t>Prunus seroti</t>
+  </si>
+  <si>
+    <t>Quercus troja</t>
+  </si>
+  <si>
+    <t>Quercus creta</t>
+  </si>
+  <si>
+    <t>Sorbus tormilis</t>
+  </si>
+  <si>
+    <t>Alnus inca</t>
+  </si>
+  <si>
+    <t>Populus xcadensis</t>
+  </si>
+  <si>
+    <t>Viburnum lanta</t>
+  </si>
+  <si>
+    <t>Paliurus spi-christi</t>
+  </si>
+  <si>
+    <t>Rubia peregri</t>
   </si>
 </sst>
 </file>
@@ -1978,7 +2017,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1994,7 +2033,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -7534,7 +7573,7 @@
         <v>132</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E40" s="13" t="s">
         <v>473</v>
@@ -9188,7 +9227,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D2" t="s">
         <v>270</v>
@@ -9372,7 +9411,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D16" t="s">
         <v>270</v>
@@ -9503,7 +9542,7 @@
         <v>26</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D26" t="s">
         <v>270</v>
@@ -9531,7 +9570,7 @@
         <v>28</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D28" t="s">
         <v>270</v>
@@ -9556,7 +9595,7 @@
         <v>30</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D30" t="s">
         <v>270</v>
@@ -9598,7 +9637,7 @@
         <v>33</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D33" t="s">
         <v>270</v>
@@ -9640,7 +9679,7 @@
         <v>36</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D36" t="s">
         <v>270</v>
@@ -9654,7 +9693,7 @@
         <v>37</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D37" t="s">
         <v>270</v>
@@ -9668,7 +9707,7 @@
         <v>38</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D38" t="s">
         <v>270</v>
@@ -9738,7 +9777,7 @@
         <v>42</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D43" t="s">
         <v>270</v>
@@ -9766,7 +9805,7 @@
         <v>44</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D45" t="s">
         <v>270</v>
@@ -9780,7 +9819,7 @@
         <v>45</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D46" t="s">
         <v>270</v>
@@ -9864,7 +9903,7 @@
         <v>51</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D52" t="s">
         <v>270</v>
@@ -9906,7 +9945,7 @@
         <v>54</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D55" t="s">
         <v>270</v>
@@ -9959,7 +9998,7 @@
         <v>58</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D59" t="s">
         <v>270</v>
@@ -9973,7 +10012,7 @@
         <v>59</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D60" t="s">
         <v>270</v>
@@ -9987,7 +10026,7 @@
         <v>60</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D61" t="s">
         <v>270</v>
@@ -10001,7 +10040,7 @@
         <v>61</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D62" t="s">
         <v>270</v>
@@ -10029,7 +10068,7 @@
         <v>63</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D64" t="s">
         <v>270</v>
@@ -10043,7 +10082,7 @@
         <v>63</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D65" t="s">
         <v>270</v>
@@ -10071,7 +10110,7 @@
         <v>65</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D67" t="s">
         <v>270</v>
@@ -10099,7 +10138,7 @@
         <v>67</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D69" t="s">
         <v>270</v>
@@ -10194,7 +10233,7 @@
         <v>73</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D76" t="s">
         <v>270</v>
@@ -10208,7 +10247,7 @@
         <v>74</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D77" t="s">
         <v>270</v>
@@ -10222,7 +10261,7 @@
         <v>75</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D78" t="s">
         <v>270</v>
@@ -10286,7 +10325,7 @@
         <v>80</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D83" t="s">
         <v>270</v>
@@ -10325,7 +10364,7 @@
         <v>83</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D86" t="s">
         <v>270</v>
@@ -10339,7 +10378,7 @@
         <v>84</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D87" t="s">
         <v>270</v>
@@ -10395,7 +10434,7 @@
         <v>88</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D91" t="s">
         <v>270</v>
@@ -10409,7 +10448,7 @@
         <v>89</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D92" t="s">
         <v>270</v>
@@ -10423,7 +10462,7 @@
         <v>90</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D93" t="s">
         <v>270</v>
@@ -10437,7 +10476,7 @@
         <v>91</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D94" t="s">
         <v>270</v>
@@ -10521,7 +10560,7 @@
         <v>95</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D100" t="s">
         <v>270</v>
@@ -10535,7 +10574,7 @@
         <v>96</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D101" t="s">
         <v>270</v>
@@ -10750,7 +10789,7 @@
         <v>112</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D117" t="s">
         <v>270</v>
@@ -10764,7 +10803,7 @@
         <v>113</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D118" t="s">
         <v>270</v>
@@ -11088,7 +11127,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D2" t="s">
         <v>270</v>
@@ -11105,7 +11144,7 @@
         <v>430</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -11152,7 +11191,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D7" t="s">
         <v>270</v>
@@ -11166,7 +11205,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D8" t="s">
         <v>270</v>
@@ -11213,7 +11252,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D12" t="s">
         <v>270</v>
@@ -11227,7 +11266,7 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D13" t="s">
         <v>270</v>
@@ -11255,10 +11294,10 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
+        <v>606</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>607</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -11269,7 +11308,7 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D16" t="s">
         <v>270</v>
@@ -11426,7 +11465,7 @@
         <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D28" t="s">
         <v>270</v>
@@ -11451,7 +11490,7 @@
         <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D30" t="s">
         <v>270</v>
@@ -11521,7 +11560,7 @@
         <v>35</v>
       </c>
       <c r="C35" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D35" t="s">
         <v>270</v>
@@ -11535,7 +11574,7 @@
         <v>36</v>
       </c>
       <c r="C36" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D36" t="s">
         <v>270</v>
@@ -11549,7 +11588,7 @@
         <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D37" t="s">
         <v>270</v>
@@ -11605,7 +11644,7 @@
         <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D41" t="s">
         <v>270</v>
@@ -11619,7 +11658,7 @@
         <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D42" t="s">
         <v>270</v>
@@ -11633,7 +11672,7 @@
         <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D43" t="s">
         <v>270</v>
@@ -11647,7 +11686,7 @@
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D44" t="s">
         <v>270</v>
@@ -11661,7 +11700,7 @@
         <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D45" t="s">
         <v>270</v>
@@ -11703,7 +11742,7 @@
         <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D48" t="s">
         <v>270</v>
@@ -11731,7 +11770,7 @@
         <v>49</v>
       </c>
       <c r="C50" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D50" t="s">
         <v>270</v>
@@ -11759,7 +11798,7 @@
         <v>51</v>
       </c>
       <c r="C52" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D52" t="s">
         <v>270</v>
@@ -11801,7 +11840,7 @@
         <v>54</v>
       </c>
       <c r="C55" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D55" t="s">
         <v>270</v>
@@ -11815,7 +11854,7 @@
         <v>55</v>
       </c>
       <c r="C56" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D56" t="s">
         <v>270</v>
@@ -11851,7 +11890,7 @@
         <v>58</v>
       </c>
       <c r="C59" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D59" t="s">
         <v>270</v>
@@ -11865,7 +11904,7 @@
         <v>59</v>
       </c>
       <c r="C60" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D60" t="s">
         <v>270</v>
@@ -11879,7 +11918,7 @@
         <v>60</v>
       </c>
       <c r="C61" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D61" t="s">
         <v>270</v>
@@ -11893,7 +11932,7 @@
         <v>61</v>
       </c>
       <c r="C62" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D62" t="s">
         <v>270</v>
@@ -11907,7 +11946,7 @@
         <v>62</v>
       </c>
       <c r="C63" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D63" t="s">
         <v>270</v>
@@ -11921,7 +11960,7 @@
         <v>63</v>
       </c>
       <c r="C64" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D64" t="s">
         <v>270</v>
@@ -11935,7 +11974,7 @@
         <v>63</v>
       </c>
       <c r="C65" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D65" t="s">
         <v>270</v>
@@ -11960,7 +11999,7 @@
         <v>65</v>
       </c>
       <c r="C67" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D67" t="s">
         <v>270</v>
@@ -11974,7 +12013,7 @@
         <v>66</v>
       </c>
       <c r="C68" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D68" t="s">
         <v>270</v>
@@ -11988,7 +12027,7 @@
         <v>67</v>
       </c>
       <c r="C69" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D69" t="s">
         <v>270</v>
@@ -12013,7 +12052,7 @@
         <v>69</v>
       </c>
       <c r="C71" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D71" t="s">
         <v>270</v>
@@ -12055,7 +12094,7 @@
         <v>71</v>
       </c>
       <c r="C74" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D74" t="s">
         <v>270</v>
@@ -12083,7 +12122,7 @@
         <v>73</v>
       </c>
       <c r="C76" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D76" t="s">
         <v>270</v>
@@ -12111,7 +12150,7 @@
         <v>75</v>
       </c>
       <c r="C78" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D78" t="s">
         <v>270</v>
@@ -12136,7 +12175,7 @@
         <v>77</v>
       </c>
       <c r="C80" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D80" t="s">
         <v>270</v>
@@ -12175,7 +12214,7 @@
         <v>80</v>
       </c>
       <c r="C83" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D83" t="s">
         <v>270</v>
@@ -12200,10 +12239,10 @@
         <v>82</v>
       </c>
       <c r="C85" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -12214,7 +12253,7 @@
         <v>83</v>
       </c>
       <c r="C86" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D86" t="s">
         <v>270</v>
@@ -12228,7 +12267,7 @@
         <v>84</v>
       </c>
       <c r="C87" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D87" t="s">
         <v>270</v>
@@ -12278,7 +12317,7 @@
         <v>88</v>
       </c>
       <c r="C91" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D91" t="s">
         <v>270</v>
@@ -12334,7 +12373,7 @@
         <v>92</v>
       </c>
       <c r="C95" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D95" t="s">
         <v>270</v>
@@ -12348,7 +12387,7 @@
         <v>92</v>
       </c>
       <c r="C96" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D96" t="s">
         <v>270</v>
@@ -12362,7 +12401,7 @@
         <v>93</v>
       </c>
       <c r="C97" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D97" t="s">
         <v>270</v>
@@ -12376,7 +12415,7 @@
         <v>93</v>
       </c>
       <c r="C98" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D98" t="s">
         <v>270</v>
@@ -12404,7 +12443,7 @@
         <v>95</v>
       </c>
       <c r="C100" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D100" t="s">
         <v>270</v>
@@ -12418,7 +12457,7 @@
         <v>96</v>
       </c>
       <c r="C101" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D101" t="s">
         <v>270</v>
@@ -12432,7 +12471,7 @@
         <v>97</v>
       </c>
       <c r="C102" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D102" t="s">
         <v>270</v>
@@ -12584,10 +12623,10 @@
         <v>108</v>
       </c>
       <c r="C113" t="s">
+        <v>602</v>
+      </c>
+      <c r="D113" s="11" t="s">
         <v>603</v>
-      </c>
-      <c r="D113" s="11" t="s">
-        <v>604</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -12623,7 +12662,7 @@
         <v>111</v>
       </c>
       <c r="C116" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D116" t="s">
         <v>270</v>
@@ -12637,7 +12676,7 @@
         <v>112</v>
       </c>
       <c r="C117" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D117" t="s">
         <v>270</v>
@@ -12704,7 +12743,7 @@
         <v>117</v>
       </c>
       <c r="C122" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D122" t="s">
         <v>270</v>
@@ -12718,7 +12757,7 @@
         <v>118</v>
       </c>
       <c r="C123" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D123" t="s">
         <v>270</v>
@@ -12732,7 +12771,7 @@
         <v>118</v>
       </c>
       <c r="C124" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D124" t="s">
         <v>270</v>
@@ -12746,7 +12785,7 @@
         <v>119</v>
       </c>
       <c r="C125" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D125" t="s">
         <v>270</v>
@@ -12763,7 +12802,7 @@
         <v>432</v>
       </c>
       <c r="D126" s="11" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -12774,7 +12813,7 @@
         <v>121</v>
       </c>
       <c r="C127" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D127" t="s">
         <v>270</v>
@@ -12788,7 +12827,7 @@
         <v>121</v>
       </c>
       <c r="C128" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D128" t="s">
         <v>270</v>
@@ -12830,7 +12869,7 @@
         <v>123</v>
       </c>
       <c r="C131" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D131" t="s">
         <v>270</v>
@@ -12844,7 +12883,7 @@
         <v>124</v>
       </c>
       <c r="C132" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D132" t="s">
         <v>270</v>
@@ -12858,7 +12897,7 @@
         <v>125</v>
       </c>
       <c r="C133" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D133" t="s">
         <v>270</v>
@@ -12872,7 +12911,7 @@
         <v>125</v>
       </c>
       <c r="C134" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D134" t="s">
         <v>270</v>
@@ -13044,7 +13083,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D7" t="s">
         <v>270</v>
@@ -13404,7 +13443,7 @@
         <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D33" t="s">
         <v>270</v>
@@ -13712,7 +13751,7 @@
         <v>54</v>
       </c>
       <c r="C55" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D55" t="s">
         <v>270</v>
@@ -13905,7 +13944,7 @@
         <v>67</v>
       </c>
       <c r="C69" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D69" t="s">
         <v>270</v>
@@ -14257,7 +14296,7 @@
         <v>92</v>
       </c>
       <c r="C95" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D95" t="s">
         <v>270</v>
@@ -14271,7 +14310,7 @@
         <v>92</v>
       </c>
       <c r="C96" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D96" t="s">
         <v>270</v>
@@ -14341,7 +14380,7 @@
         <v>96</v>
       </c>
       <c r="C101" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D101" t="s">
         <v>270</v>
@@ -14887,7 +14926,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D2" t="s">
         <v>270</v>
@@ -15267,7 +15306,7 @@
         <v>30</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D30" t="s">
         <v>270</v>
@@ -15309,7 +15348,7 @@
         <v>33</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D33" t="s">
         <v>270</v>
@@ -15491,7 +15530,7 @@
         <v>45</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D46" t="s">
         <v>270</v>
@@ -15575,7 +15614,7 @@
         <v>51</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D52" t="s">
         <v>270</v>
@@ -15617,7 +15656,7 @@
         <v>54</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D55" t="s">
         <v>270</v>
@@ -15695,7 +15734,7 @@
         <v>60</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D61" t="s">
         <v>270</v>
@@ -15737,7 +15776,7 @@
         <v>63</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D64" t="s">
         <v>270</v>
@@ -15751,7 +15790,7 @@
         <v>63</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D65" t="s">
         <v>270</v>
@@ -15776,7 +15815,7 @@
         <v>65</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D67" t="s">
         <v>270</v>
@@ -16131,7 +16170,7 @@
         <v>90</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D93" t="s">
         <v>270</v>
@@ -16145,7 +16184,7 @@
         <v>91</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D94" t="s">
         <v>270</v>
@@ -16187,7 +16226,7 @@
         <v>93</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D97" t="s">
         <v>270</v>
@@ -16201,7 +16240,7 @@
         <v>93</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D98" t="s">
         <v>270</v>
@@ -16215,7 +16254,7 @@
         <v>94</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D99" t="s">
         <v>270</v>
@@ -16573,7 +16612,7 @@
         <v>119</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D125" t="s">
         <v>270</v>
@@ -16770,7 +16809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{813A7B90-BA19-4A62-A054-1665FB26E5CE}">
   <dimension ref="A1:I138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
       <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
@@ -16791,7 +16830,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>608</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>487</v>
@@ -16823,16 +16862,16 @@
         <v>2</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>294</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>149</v>
@@ -16840,9 +16879,7 @@
       <c r="H2" s="11" t="s">
         <v>493</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -16863,15 +16900,9 @@
       <c r="F3" s="11" t="s">
         <v>430</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -16898,9 +16929,7 @@
       <c r="H4" s="11" t="s">
         <v>493</v>
       </c>
-      <c r="I4" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -16918,18 +16947,14 @@
       <c r="E5" s="11" t="s">
         <v>308</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="F5" s="6"/>
       <c r="G5" s="6" t="s">
         <v>151</v>
       </c>
       <c r="H5" s="11" t="s">
         <v>493</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -16947,18 +16972,12 @@
       <c r="E6" s="11" t="s">
         <v>295</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="F6" s="6"/>
       <c r="G6" s="6" t="s">
         <v>469</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -16974,10 +16993,10 @@
         <v>330</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>152</v>
@@ -17006,7 +17025,7 @@
         <v>296</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>153</v>
@@ -17023,29 +17042,19 @@
         <v>44</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>496</v>
-      </c>
+        <v>609</v>
+      </c>
+      <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
         <v>440</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>321</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -17054,27 +17063,15 @@
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -17083,34 +17080,22 @@
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
       <c r="E11" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>47</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>610</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>228</v>
@@ -17122,24 +17107,20 @@
         <v>297</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="H12" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>48</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>611</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>229</v>
@@ -17151,7 +17132,7 @@
         <v>294</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>155</v>
@@ -17159,9 +17140,7 @@
       <c r="H13" s="11" t="s">
         <v>493</v>
       </c>
-      <c r="I13" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -17188,9 +17167,7 @@
       <c r="H14" s="11" t="s">
         <v>493</v>
       </c>
-      <c r="I14" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -17199,9 +17176,7 @@
       <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="C15" s="6"/>
       <c r="D15" s="6" t="s">
         <v>441</v>
       </c>
@@ -17209,17 +17184,11 @@
         <v>317</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>607</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>496</v>
-      </c>
+        <v>606</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -17229,7 +17198,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>333</v>
@@ -17238,7 +17207,7 @@
         <v>297</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>158</v>
@@ -17272,12 +17241,8 @@
       <c r="G17" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="H17" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -17304,9 +17269,7 @@
       <c r="H18" s="11" t="s">
         <v>493</v>
       </c>
-      <c r="I18" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="I18" s="6"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -17315,27 +17278,13 @@
       <c r="B19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -17362,9 +17311,7 @@
       <c r="H20" s="11" t="s">
         <v>493</v>
       </c>
-      <c r="I20" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="I20" s="6"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -17373,34 +17320,26 @@
       <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="C21" s="6"/>
       <c r="D21" s="6" t="s">
         <v>357</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>321</v>
       </c>
-      <c r="F21" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="F21" s="6"/>
       <c r="G21" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="H21" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>70</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>22</v>
+        <v>612</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>252</v>
@@ -17411,18 +17350,14 @@
       <c r="E22" s="11" t="s">
         <v>317</v>
       </c>
-      <c r="F22" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="F22" s="6"/>
       <c r="G22" s="6" t="s">
         <v>162</v>
       </c>
       <c r="H22" s="11" t="s">
         <v>493</v>
       </c>
-      <c r="I22" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -17449,9 +17384,7 @@
       <c r="H23" s="11" t="s">
         <v>493</v>
       </c>
-      <c r="I23" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="I23" s="6"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
@@ -17460,27 +17393,19 @@
       <c r="B24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="C24" s="6"/>
       <c r="D24" s="6" t="s">
         <v>354</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="F24" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="F24" s="6"/>
       <c r="G24" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="H24" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
@@ -17507,9 +17432,7 @@
       <c r="H25" s="11" t="s">
         <v>493</v>
       </c>
-      <c r="I25" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="I25" s="6"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
@@ -17519,7 +17442,7 @@
         <v>26</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>366</v>
@@ -17536,9 +17459,7 @@
       <c r="H26" s="11" t="s">
         <v>493</v>
       </c>
-      <c r="I26" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="I26" s="6"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
@@ -17577,7 +17498,7 @@
         <v>28</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>335</v>
@@ -17586,7 +17507,7 @@
         <v>298</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>166</v>
@@ -17605,27 +17526,13 @@
       <c r="B29" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
@@ -17635,16 +17542,16 @@
         <v>30</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>296</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>167</v>
@@ -17722,13 +17629,13 @@
         <v>33</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F33" s="11" t="s">
         <v>276</v>
@@ -17765,12 +17672,8 @@
       <c r="G34" s="6" t="s">
         <v>398</v>
       </c>
-      <c r="H34" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="I34" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
@@ -17789,7 +17692,7 @@
         <v>316</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>170</v>
@@ -17809,7 +17712,7 @@
         <v>36</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>338</v>
@@ -17818,7 +17721,7 @@
         <v>316</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>157</v>
@@ -17838,7 +17741,7 @@
         <v>37</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>339</v>
@@ -17847,11 +17750,9 @@
         <v>299</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>527</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>496</v>
-      </c>
+        <v>526</v>
+      </c>
+      <c r="G37" s="6"/>
       <c r="H37" s="11" t="s">
         <v>137</v>
       </c>
@@ -17867,7 +17768,7 @@
         <v>38</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>340</v>
@@ -17937,7 +17838,7 @@
         <v>279</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="H40" s="11" t="s">
         <v>137</v>
@@ -17963,7 +17864,7 @@
         <v>308</v>
       </c>
       <c r="F41" s="11" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>173</v>
@@ -17971,9 +17872,7 @@
       <c r="H41" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="I41" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="I41" s="6"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
@@ -17992,7 +17891,7 @@
         <v>308</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>173</v>
@@ -18000,9 +17899,7 @@
       <c r="H42" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="I42" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="I42" s="6"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
@@ -18012,7 +17909,7 @@
         <v>42</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>343</v>
@@ -18021,7 +17918,7 @@
         <v>295</v>
       </c>
       <c r="F43" s="11" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>174</v>
@@ -18050,7 +17947,7 @@
         <v>309</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="G44" s="6" t="s">
         <v>176</v>
@@ -18070,7 +17967,7 @@
         <v>44</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>345</v>
@@ -18079,7 +17976,7 @@
         <v>310</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="G45" s="6" t="s">
         <v>177</v>
@@ -18099,10 +17996,10 @@
         <v>45</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E46" s="11" t="s">
         <v>272</v>
@@ -18125,7 +18022,7 @@
         <v>293</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>46</v>
+        <v>613</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>334</v>
@@ -18166,7 +18063,7 @@
         <v>312</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G48" s="6" t="s">
         <v>179</v>
@@ -18224,11 +18121,9 @@
         <v>302</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>533</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>496</v>
-      </c>
+        <v>532</v>
+      </c>
+      <c r="G50" s="6"/>
       <c r="H50" s="11" t="s">
         <v>139</v>
       </c>
@@ -18273,16 +18168,16 @@
         <v>51</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E52" s="11" t="s">
         <v>299</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="G52" s="6" t="s">
         <v>182</v>
@@ -18299,7 +18194,7 @@
         <v>303</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>52</v>
+        <v>614</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>244</v>
@@ -18313,9 +18208,7 @@
       <c r="F53" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="G53" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="G53" s="6"/>
       <c r="H53" s="11" t="s">
         <v>139</v>
       </c>
@@ -18360,16 +18253,16 @@
         <v>54</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F55" s="11" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="G55" s="6" t="s">
         <v>391</v>
@@ -18398,7 +18291,7 @@
         <v>301</v>
       </c>
       <c r="F56" s="11" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G56" s="6" t="s">
         <v>184</v>
@@ -18417,56 +18310,32 @@
       <c r="B57" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C57" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="G57" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="H57" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="I57" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>310</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>57</v>
+        <v>615</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="D58" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="D58" s="6"/>
       <c r="E58" s="11" t="s">
         <v>299</v>
       </c>
-      <c r="F58" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="G58" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="H58" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="I58" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
@@ -18476,7 +18345,7 @@
         <v>58</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>351</v>
@@ -18485,7 +18354,7 @@
         <v>302</v>
       </c>
       <c r="F59" s="11" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G59" s="6" t="s">
         <v>185</v>
@@ -18505,7 +18374,7 @@
         <v>59</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>351</v>
@@ -18514,7 +18383,7 @@
         <v>302</v>
       </c>
       <c r="F60" s="11" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G60" s="6" t="s">
         <v>185</v>
@@ -18531,19 +18400,19 @@
         <v>320</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>60</v>
+        <v>616</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E61" s="11" t="s">
         <v>301</v>
       </c>
       <c r="F61" s="11" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="G61" s="6" t="s">
         <v>186</v>
@@ -18563,7 +18432,7 @@
         <v>61</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>448</v>
@@ -18572,7 +18441,7 @@
         <v>299</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="G62" s="6" t="s">
         <v>187</v>
@@ -18601,11 +18470,9 @@
         <v>315</v>
       </c>
       <c r="F63" s="11" t="s">
-        <v>540</v>
-      </c>
-      <c r="G63" s="6" t="s">
-        <v>496</v>
-      </c>
+        <v>539</v>
+      </c>
+      <c r="G63" s="6"/>
       <c r="H63" s="11" t="s">
         <v>140</v>
       </c>
@@ -18621,16 +18488,16 @@
         <v>63</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E64" s="11" t="s">
         <v>327</v>
       </c>
       <c r="F64" s="11" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="G64" s="6" t="s">
         <v>188</v>
@@ -18650,16 +18517,16 @@
         <v>63</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E65" s="11" t="s">
         <v>327</v>
       </c>
       <c r="F65" s="11" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="G65" s="6" t="s">
         <v>188</v>
@@ -18681,18 +18548,12 @@
       <c r="C66" s="6" t="s">
         <v>374</v>
       </c>
-      <c r="D66" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="D66" s="6"/>
       <c r="E66" s="11" t="s">
         <v>299</v>
       </c>
-      <c r="F66" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="G66" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
       <c r="H66" s="11" t="s">
         <v>140</v>
       </c>
@@ -18708,16 +18569,16 @@
         <v>65</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E67" s="11" t="s">
         <v>305</v>
       </c>
       <c r="F67" s="11" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G67" s="6" t="s">
         <v>189</v>
@@ -18746,7 +18607,7 @@
         <v>295</v>
       </c>
       <c r="F68" s="11" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="G68" s="6" t="s">
         <v>196</v>
@@ -18766,16 +18627,16 @@
         <v>67</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>448</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F69" s="11" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="G69" s="6" t="s">
         <v>182</v>
@@ -18794,18 +18655,12 @@
       <c r="B70" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C70" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
       <c r="E70" s="11" t="s">
         <v>326</v>
       </c>
-      <c r="F70" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="F70" s="6"/>
       <c r="G70" s="6" t="s">
         <v>474</v>
       </c>
@@ -18833,7 +18688,7 @@
         <v>298</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G71" s="6" t="s">
         <v>190</v>
@@ -18858,15 +18713,11 @@
       <c r="D72" s="6" t="s">
         <v>448</v>
       </c>
-      <c r="E72" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="E72" s="6"/>
       <c r="F72" s="11" t="s">
         <v>431</v>
       </c>
-      <c r="G72" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="G72" s="6"/>
       <c r="H72" s="11" t="s">
         <v>140</v>
       </c>
@@ -18887,15 +18738,11 @@
       <c r="D73" s="6" t="s">
         <v>448</v>
       </c>
-      <c r="E73" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="E73" s="6"/>
       <c r="F73" s="11" t="s">
         <v>431</v>
       </c>
-      <c r="G73" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="G73" s="6"/>
       <c r="H73" s="11" t="s">
         <v>140</v>
       </c>
@@ -18920,7 +18767,7 @@
         <v>310</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G74" s="6" t="s">
         <v>191</v>
@@ -18954,12 +18801,8 @@
       <c r="G75" s="6" t="s">
         <v>476</v>
       </c>
-      <c r="H75" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="I75" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
@@ -18969,7 +18812,7 @@
         <v>73</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>357</v>
@@ -18978,7 +18821,7 @@
         <v>308</v>
       </c>
       <c r="F76" s="11" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G76" s="6" t="s">
         <v>464</v>
@@ -18998,7 +18841,7 @@
         <v>74</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D77" s="6" t="s">
         <v>245</v>
@@ -19024,10 +18867,10 @@
         <v>400</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>75</v>
+        <v>617</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>358</v>
@@ -19036,7 +18879,7 @@
         <v>295</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G78" s="6" t="s">
         <v>192</v>
@@ -19064,18 +18907,14 @@
       <c r="E79" s="11" t="s">
         <v>317</v>
       </c>
-      <c r="F79" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="F79" s="6"/>
       <c r="G79" s="6" t="s">
         <v>193</v>
       </c>
       <c r="H79" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="I79" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="I79" s="6"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
@@ -19094,7 +18933,7 @@
         <v>321</v>
       </c>
       <c r="F80" s="11" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="G80" s="6" t="s">
         <v>194</v>
@@ -19113,27 +18952,19 @@
       <c r="B81" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C81" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="C81" s="6"/>
       <c r="D81" s="6" t="s">
         <v>360</v>
       </c>
-      <c r="E81" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="E81" s="6"/>
       <c r="F81" s="11" t="s">
         <v>415</v>
       </c>
-      <c r="G81" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="G81" s="6"/>
       <c r="H81" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="I81" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="I81" s="6"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
@@ -19142,27 +18973,17 @@
       <c r="B82" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C82" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="C82" s="6"/>
       <c r="D82" s="6" t="s">
         <v>313</v>
       </c>
       <c r="E82" s="11" t="s">
         <v>322</v>
       </c>
-      <c r="F82" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="G82" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="H82" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="I82" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
@@ -19172,7 +18993,7 @@
         <v>80</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>361</v>
@@ -19181,17 +19002,13 @@
         <v>297</v>
       </c>
       <c r="F83" s="11" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G83" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="H83" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="I83" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
@@ -19200,46 +19017,30 @@
       <c r="B84" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C84" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="E84" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="F84" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="G84" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="H84" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="I84" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="6"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>422</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>82</v>
+        <v>618</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>444</v>
       </c>
-      <c r="D85" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="D85" s="6"/>
       <c r="E85" s="11" t="s">
         <v>317</v>
       </c>
       <c r="F85" s="11" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="G85" s="6" t="s">
         <v>196</v>
@@ -19259,7 +19060,7 @@
         <v>83</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>362</v>
@@ -19268,7 +19069,7 @@
         <v>318</v>
       </c>
       <c r="F86" s="11" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="G86" s="6" t="s">
         <v>197</v>
@@ -19288,7 +19089,7 @@
         <v>84</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D87" s="6" t="s">
         <v>252</v>
@@ -19297,7 +19098,7 @@
         <v>319</v>
       </c>
       <c r="F87" s="11" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="G87" s="6" t="s">
         <v>198</v>
@@ -19325,9 +19126,7 @@
       <c r="E88" s="11" t="s">
         <v>324</v>
       </c>
-      <c r="F88" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="F88" s="6"/>
       <c r="G88" s="6" t="s">
         <v>170</v>
       </c>
@@ -19354,12 +19153,8 @@
       <c r="E89" s="11" t="s">
         <v>308</v>
       </c>
-      <c r="F89" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="G89" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
       <c r="H89" s="11" t="s">
         <v>137</v>
       </c>
@@ -19404,7 +19199,7 @@
         <v>88</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D91" s="6" t="s">
         <v>361</v>
@@ -19413,7 +19208,7 @@
         <v>320</v>
       </c>
       <c r="F91" s="11" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="G91" s="6" t="s">
         <v>200</v>
@@ -19433,7 +19228,7 @@
         <v>89</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D92" s="6" t="s">
         <v>361</v>
@@ -19462,10 +19257,10 @@
         <v>90</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E93" s="11" t="s">
         <v>311</v>
@@ -19491,10 +19286,10 @@
         <v>91</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E94" s="11" t="s">
         <v>319</v>
@@ -19526,10 +19321,10 @@
         <v>366</v>
       </c>
       <c r="E95" s="11" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F95" s="11" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="G95" s="6" t="s">
         <v>204</v>
@@ -19555,10 +19350,10 @@
         <v>366</v>
       </c>
       <c r="E96" s="11" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F96" s="11" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="G96" s="6" t="s">
         <v>204</v>
@@ -19581,13 +19376,13 @@
         <v>254</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E97" s="11" t="s">
         <v>295</v>
       </c>
       <c r="F97" s="11" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="G97" s="6" t="s">
         <v>205</v>
@@ -19610,13 +19405,13 @@
         <v>254</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E98" s="11" t="s">
         <v>295</v>
       </c>
       <c r="F98" s="11" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="G98" s="6" t="s">
         <v>205</v>
@@ -19639,7 +19434,7 @@
         <v>255</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E99" s="11" t="s">
         <v>300</v>
@@ -19665,7 +19460,7 @@
         <v>95</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>334</v>
@@ -19674,7 +19469,7 @@
         <v>308</v>
       </c>
       <c r="F100" s="11" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="G100" s="6" t="s">
         <v>206</v>
@@ -19682,9 +19477,7 @@
       <c r="H100" s="11" t="s">
         <v>493</v>
       </c>
-      <c r="I100" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="I100" s="6"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
@@ -19694,16 +19487,16 @@
         <v>96</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D101" s="6" t="s">
         <v>352</v>
       </c>
       <c r="E101" s="11" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F101" s="11" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="G101" s="15" t="s">
         <v>492</v>
@@ -19732,17 +19525,11 @@
         <v>323</v>
       </c>
       <c r="F102" s="11" t="s">
-        <v>558</v>
-      </c>
-      <c r="G102" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="H102" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="I102" s="6" t="s">
-        <v>496</v>
-      </c>
+        <v>557</v>
+      </c>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
@@ -19786,15 +19573,11 @@
       <c r="D104" s="6" t="s">
         <v>452</v>
       </c>
-      <c r="E104" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="E104" s="6"/>
       <c r="F104" s="11" t="s">
         <v>419</v>
       </c>
-      <c r="G104" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="G104" s="6"/>
       <c r="H104" s="11" t="s">
         <v>140</v>
       </c>
@@ -19809,9 +19592,7 @@
       <c r="B105" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C105" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="C105" s="6"/>
       <c r="D105" s="6" t="s">
         <v>353</v>
       </c>
@@ -19847,9 +19628,7 @@
       <c r="E106" s="11" t="s">
         <v>298</v>
       </c>
-      <c r="F106" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="F106" s="6"/>
       <c r="G106" s="6" t="s">
         <v>159</v>
       </c>
@@ -19865,7 +19644,7 @@
         <v>605</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>102</v>
+        <v>619</v>
       </c>
       <c r="C107" s="6" t="s">
         <v>240</v>
@@ -19896,15 +19675,11 @@
       <c r="B108" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C108" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="C108" s="6"/>
       <c r="D108" s="6" t="s">
         <v>453</v>
       </c>
-      <c r="E108" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="E108" s="6"/>
       <c r="F108" s="11" t="s">
         <v>422</v>
       </c>
@@ -19981,7 +19756,7 @@
         <v>620</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>106</v>
+        <v>620</v>
       </c>
       <c r="C111" s="6" t="s">
         <v>374</v>
@@ -19989,9 +19764,7 @@
       <c r="D111" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="E111" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="E111" s="6"/>
       <c r="F111" s="11" t="s">
         <v>280</v>
       </c>
@@ -20015,9 +19788,7 @@
       <c r="C112" s="6" t="s">
         <v>374</v>
       </c>
-      <c r="D112" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="D112" s="6"/>
       <c r="E112" s="11" t="s">
         <v>325</v>
       </c>
@@ -20047,15 +19818,11 @@
       <c r="D113" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="E113" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="E113" s="6"/>
       <c r="F113" s="11" t="s">
-        <v>603</v>
-      </c>
-      <c r="G113" s="6" t="s">
-        <v>496</v>
-      </c>
+        <v>602</v>
+      </c>
+      <c r="G113" s="6"/>
       <c r="H113" s="11" t="s">
         <v>137</v>
       </c>
@@ -20070,21 +19837,13 @@
       <c r="B114" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C114" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="D114" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="C114" s="6"/>
+      <c r="D114" s="6"/>
       <c r="E114" s="11" t="s">
         <v>300</v>
       </c>
-      <c r="F114" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="G114" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="F114" s="6"/>
+      <c r="G114" s="6"/>
       <c r="H114" s="11" t="s">
         <v>137</v>
       </c>
@@ -20111,9 +19870,7 @@
       <c r="F115" s="11" t="s">
         <v>290</v>
       </c>
-      <c r="G115" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="G115" s="6"/>
       <c r="H115" s="11" t="s">
         <v>140</v>
       </c>
@@ -20138,7 +19895,7 @@
         <v>310</v>
       </c>
       <c r="F116" s="11" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="G116" s="6" t="s">
         <v>213</v>
@@ -20158,7 +19915,7 @@
         <v>112</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D117" s="6" t="s">
         <v>363</v>
@@ -20167,7 +19924,7 @@
         <v>322</v>
       </c>
       <c r="F117" s="11" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="G117" s="6" t="s">
         <v>165</v>
@@ -20187,20 +19944,16 @@
         <v>113</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D118" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="E118" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="E118" s="6"/>
       <c r="F118" s="11" t="s">
         <v>427</v>
       </c>
-      <c r="G118" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="G118" s="6"/>
       <c r="H118" s="11" t="s">
         <v>137</v>
       </c>
@@ -20244,18 +19997,14 @@
       <c r="B120" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C120" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="C120" s="6"/>
       <c r="D120" s="6" t="s">
         <v>456</v>
       </c>
       <c r="E120" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="F120" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="F120" s="6"/>
       <c r="G120" s="6" t="s">
         <v>214</v>
       </c>
@@ -20312,7 +20061,7 @@
         <v>325</v>
       </c>
       <c r="F122" s="11" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="G122" s="6" t="s">
         <v>216</v>
@@ -20341,7 +20090,7 @@
         <v>305</v>
       </c>
       <c r="F123" s="11" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G123" s="6" t="s">
         <v>217</v>
@@ -20370,7 +20119,7 @@
         <v>305</v>
       </c>
       <c r="F124" s="11" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G124" s="6" t="s">
         <v>217</v>
@@ -20393,13 +20142,13 @@
         <v>263</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E125" s="11" t="s">
         <v>306</v>
       </c>
       <c r="F125" s="11" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G125" s="6" t="s">
         <v>218</v>
@@ -20421,18 +20170,12 @@
       <c r="C126" s="6" t="s">
         <v>375</v>
       </c>
-      <c r="D126" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="E126" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="D126" s="6"/>
+      <c r="E126" s="6"/>
       <c r="F126" s="11" t="s">
         <v>432</v>
       </c>
-      <c r="G126" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="G126" s="6"/>
       <c r="H126" s="11" t="s">
         <v>140</v>
       </c>
@@ -20457,7 +20200,7 @@
         <v>308</v>
       </c>
       <c r="F127" s="11" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G127" s="6" t="s">
         <v>219</v>
@@ -20486,7 +20229,7 @@
         <v>308</v>
       </c>
       <c r="F128" s="11" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G128" s="6" t="s">
         <v>219</v>
@@ -20573,7 +20316,7 @@
         <v>298</v>
       </c>
       <c r="F131" s="11" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="G131" s="6" t="s">
         <v>221</v>
@@ -20602,7 +20345,7 @@
         <v>303</v>
       </c>
       <c r="F132" s="11" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="G132" s="6" t="s">
         <v>200</v>
@@ -20631,7 +20374,7 @@
         <v>328</v>
       </c>
       <c r="F133" s="11" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="G133" s="6" t="s">
         <v>222</v>
@@ -20660,7 +20403,7 @@
         <v>328</v>
       </c>
       <c r="F134" s="11" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="G134" s="6" t="s">
         <v>222</v>
@@ -20679,27 +20422,19 @@
       <c r="B135" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C135" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="C135" s="6"/>
       <c r="D135" s="6" t="s">
         <v>445</v>
       </c>
       <c r="E135" s="11" t="s">
         <v>295</v>
       </c>
-      <c r="F135" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="G135" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="F135" s="6"/>
+      <c r="G135" s="6"/>
       <c r="H135" s="11" t="s">
         <v>494</v>
       </c>
-      <c r="I135" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="I135" s="6"/>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
@@ -20708,34 +20443,22 @@
       <c r="B136" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C136" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="D136" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="E136" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="F136" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="C136" s="6"/>
+      <c r="D136" s="6"/>
+      <c r="E136" s="6"/>
+      <c r="F136" s="6"/>
       <c r="G136" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="H136" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="I136" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="H136" s="6"/>
+      <c r="I136" s="6"/>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>774</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>128</v>
+        <v>621</v>
       </c>
       <c r="C137" s="6" t="s">
         <v>359</v>
@@ -20743,15 +20466,11 @@
       <c r="D137" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="E137" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="E137" s="6"/>
       <c r="F137" s="11" t="s">
         <v>428</v>
       </c>
-      <c r="G137" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="G137" s="6"/>
       <c r="H137" s="11" t="s">
         <v>137</v>
       </c>
@@ -20766,21 +20485,13 @@
       <c r="B138" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C138" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="C138" s="6"/>
       <c r="D138" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="E138" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="F138" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="G138" s="6" t="s">
-        <v>496</v>
-      </c>
+      <c r="E138" s="6"/>
+      <c r="F138" s="6"/>
+      <c r="G138" s="6"/>
       <c r="H138" s="11" t="s">
         <v>140</v>
       </c>

</xml_diff>